<commit_message>
:pencil: Update June 2022
</commit_message>
<xml_diff>
--- a/Data/excel/nic2019-20220418.xlsx
+++ b/Data/excel/nic2019-20220418.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifyou\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifyou\Documents\GitHub\migrants_usbp\Data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72484A71-F871-40E9-92E0-10E779766EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B99D07-0FD7-4FA5-BF47-EE69167651B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -246,9 +246,6 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
@@ -624,7 +621,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:M8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -685,14 +682,14 @@
       <c r="A2">
         <v>2022</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="17">
         <v>9305</v>
       </c>
       <c r="C2" s="4">
-        <v>13679</v>
+        <v>13680</v>
       </c>
       <c r="D2" s="4">
-        <v>15337</v>
+        <v>15336</v>
       </c>
       <c r="E2" s="5">
         <v>11637</v>
@@ -701,53 +698,59 @@
         <v>13358</v>
       </c>
       <c r="G2" s="6">
-        <v>16085</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+        <v>16087</v>
+      </c>
+      <c r="H2" s="6">
+        <v>12635</v>
+      </c>
+      <c r="I2" s="6">
+        <v>19080</v>
+      </c>
+      <c r="J2" s="6">
+        <v>11258</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2021</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>314</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>446</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>708</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>575</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>748</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>1990</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>3120</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>4451</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>7472</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="12">
         <v>13509</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <v>10024</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <v>7365</v>
       </c>
     </row>
@@ -755,40 +758,40 @@
       <c r="A4">
         <v>2020</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>427</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>396</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>379</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>301</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>303</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>320</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>120</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <v>149</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <v>134</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="14">
         <v>153</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>211</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>271</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:pencil: Update Aug 2022
</commit_message>
<xml_diff>
--- a/Data/excel/nic2019-20220418.xlsx
+++ b/Data/excel/nic2019-20220418.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifyou\Documents\GitHub\migrants_usbp\Data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B99D07-0FD7-4FA5-BF47-EE69167651B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D0AF0-0681-4166-9487-BA354365CAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -621,7 +634,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -686,7 +699,7 @@
         <v>9305</v>
       </c>
       <c r="C2" s="4">
-        <v>13680</v>
+        <v>13679</v>
       </c>
       <c r="D2" s="4">
         <v>15336</v>
@@ -695,22 +708,26 @@
         <v>11637</v>
       </c>
       <c r="F2" s="4">
-        <v>13358</v>
+        <v>13357</v>
       </c>
       <c r="G2" s="6">
-        <v>16087</v>
+        <v>16085</v>
       </c>
       <c r="H2" s="6">
-        <v>12635</v>
+        <v>12634</v>
       </c>
       <c r="I2" s="6">
-        <v>19080</v>
+        <v>19088</v>
       </c>
       <c r="J2" s="6">
-        <v>11258</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+        <v>11254</v>
+      </c>
+      <c r="K2" s="6">
+        <v>12130</v>
+      </c>
+      <c r="L2" s="6">
+        <v>11825</v>
+      </c>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
:pencil: Updated Jan 2024
</commit_message>
<xml_diff>
--- a/Data/excel/nic2019-20220418.xlsx
+++ b/Data/excel/nic2019-20220418.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ifyou\Documents\GitHub\migrants_usbp\Data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D0AF0-0681-4166-9487-BA354365CAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A06128-CA90-4442-9C59-2ADA5532822C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>